<commit_message>
updated file bugreports and checklist
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nazar\Desktop\SwagLabs-QA-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4407729B-EF2E-4D39-8ABD-FACEC79D78B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FB1C8B-3F02-4BF3-83A6-A5AC43BC3CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -120,12 +120,6 @@
     <t>I05</t>
   </si>
   <si>
-    <t>Verify all product images are loaded</t>
-  </si>
-  <si>
-    <t>Verify sorting "Name (Z to A)"</t>
-  </si>
-  <si>
     <t>Verify sorting "Price (low to high)"</t>
   </si>
   <si>
@@ -204,17 +198,68 @@
     <t>https://www.saucedemo.com/</t>
   </si>
   <si>
-    <t>Burger menu overlaps items</t>
-  </si>
-  <si>
     <t>Project: Swag Labs (SauceDemo)</t>
+  </si>
+  <si>
+    <t>Layout is correct</t>
+  </si>
+  <si>
+    <t>I06</t>
+  </si>
+  <si>
+    <t>Verify product images display correctly (problem_user)</t>
+  </si>
+  <si>
+    <r>
+      <t>Bug FUNC-001:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Dog placeholders shown</t>
+    </r>
+  </si>
+  <si>
+    <t>All images match products</t>
+  </si>
+  <si>
+    <t>I07</t>
+  </si>
+  <si>
+    <t>Verify sorting "Name (Z to A)" (problem_user)</t>
+  </si>
+  <si>
+    <r>
+      <t>Bug FUNC-002:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Items do not reorder</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify all product images display correctly (standard_user)</t>
+  </si>
+  <si>
+    <t>Verify sorting "Name (Z to A)" (standard_user)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +277,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -281,7 +334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -418,11 +471,41 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -432,7 +515,20 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -443,7 +539,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -459,23 +555,27 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -757,16 +857,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E23" activeCellId="1" sqref="B17 E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.765625" customWidth="1"/>
-    <col min="2" max="2" width="48.3046875" customWidth="1"/>
+    <col min="2" max="2" width="49.15234375" customWidth="1"/>
     <col min="3" max="3" width="7.765625" customWidth="1"/>
     <col min="4" max="4" width="7.69140625" customWidth="1"/>
     <col min="5" max="5" width="39.53515625" customWidth="1"/>
@@ -779,7 +879,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -795,17 +895,17 @@
         <v>4</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -814,18 +914,18 @@
       <c r="C2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="31" t="s">
-        <v>58</v>
+      <c r="H2" s="24" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -834,7 +934,7 @@
       <c r="C3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -842,7 +942,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -851,7 +951,7 @@
       <c r="C4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -859,7 +959,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -868,7 +968,7 @@
       <c r="C5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -876,7 +976,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -885,7 +985,7 @@
       <c r="C6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -893,210 +993,246 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>31</v>
+      <c r="B7" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="4"/>
+      <c r="D7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>32</v>
+      <c r="B8" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>33</v>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>34</v>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="B14" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
+      <c r="D14" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="27"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>51</v>
-      </c>
+      <c r="D15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
-        <v>49</v>
+      <c r="A16" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="21" t="s">
+      <c r="D16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A18" s="25" t="s">
+      <c r="B20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="26" t="s">
+      <c r="D20" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C21" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="23" t="s">
         <v>55</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new file TestCases.md
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nazar\Desktop\SwagLabs-QA-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FB1C8B-3F02-4BF3-83A6-A5AC43BC3CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470CDA23-12ED-44CE-B7DA-616B7FB9E3A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -860,7 +860,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" activeCellId="1" sqref="B17 E23"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>